<commit_message>
Additional calibration edit for EV sales
</commit_message>
<xml_diff>
--- a/InputData/trans/BBSoEVP/BBSoEVP BAU Battery Share of Electric Vehicle Price.xlsx
+++ b/InputData/trans/BBSoEVP/BBSoEVP BAU Battery Share of Electric Vehicle Price.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BBSoEVP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75D70FC-5F56-46D4-B322-CE729ED16872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DCA6D8-4FE0-44AC-84F7-E2AC8163ACBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2165,7 +2165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
@@ -14960,8 +14960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A9DD83-4E8C-4A41-986C-F727F17C4502}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15235,7 +15235,7 @@
         <v>68</v>
       </c>
       <c r="B25">
-        <v>38847.800000000003</v>
+        <v>39190.400000000001</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
@@ -15243,7 +15243,7 @@
         <v>69</v>
       </c>
       <c r="B26">
-        <v>33166.400000000001</v>
+        <v>32444.6</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -15252,7 +15252,7 @@
       </c>
       <c r="B27" s="4">
         <f>1-B25/B24</f>
-        <v>0.22298183854708375</v>
+        <v>0.21612929034322748</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
@@ -15261,7 +15261,7 @@
       </c>
       <c r="B28" s="4">
         <f>1-B26/B24</f>
-        <v>0.33661892951436112</v>
+        <v>0.35105608448675896</v>
       </c>
     </row>
   </sheetData>
@@ -15278,8 +15278,8 @@
   </sheetPr>
   <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:AG7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15394,126 +15394,124 @@
         <v>4</v>
       </c>
       <c r="B2" s="5">
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="C2" s="5">
-        <f>B2+($H$2-$B$2)/COUNT($C$1:$H$1)</f>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="D2" s="5">
-        <f t="shared" ref="D2:G2" si="0">C2+($H$2-$B$2)/COUNT($C$1:$H$1)</f>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="E2" s="5">
+        <v>0.44</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0.44</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0.44</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0.44</v>
+      </c>
+      <c r="I2" s="5">
+        <f>H2+($M$2-$H$2)/COUNT($I$1:$M$1)</f>
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="J2" s="5">
+        <f t="shared" ref="J2:K2" si="0">I2+($M$2-$H$2)/COUNT($I$1:$M$1)</f>
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="K2" s="5">
         <f t="shared" si="0"/>
-        <v>0.35</v>
-      </c>
-      <c r="F2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.35</v>
-      </c>
-      <c r="G2" s="5">
-        <f t="shared" si="0"/>
-        <v>0.35</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0.35</v>
-      </c>
-      <c r="I2" s="5">
-        <f>0.37</f>
-        <v>0.37</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0.39</v>
-      </c>
-      <c r="K2" s="5">
-        <v>0.41</v>
+        <v>0.47600000000000003</v>
       </c>
       <c r="L2" s="5">
-        <v>0.43</v>
+        <f>K2+($M$2-$H$2)/COUNT($I$1:$M$1)</f>
+        <v>0.48800000000000004</v>
       </c>
       <c r="M2" s="5">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="N2" s="5">
         <f t="shared" ref="N2:AG2" si="1">M2</f>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="O2" s="5">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="P2" s="5">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="Q2" s="5">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="R2" s="5">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="S2" s="5">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="T2" s="5">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="U2" s="5">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="V2" s="5">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="W2" s="5">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="X2" s="5">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="Y2" s="5">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="Z2" s="5">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AA2" s="5">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AB2" s="5">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AC2" s="5">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AD2" s="5">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AE2" s="5">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AF2" s="5">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AG2" s="5">
         <f t="shared" si="1"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.35">
@@ -15522,131 +15520,131 @@
       </c>
       <c r="B3" s="5">
         <f>B2</f>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="C3" s="5">
         <f t="shared" ref="C3:AG7" si="2">C2</f>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="D3" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="E3" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="F3" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="G3" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="H3" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="I3" s="5">
         <f t="shared" si="2"/>
-        <v>0.37</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" si="2"/>
-        <v>0.39</v>
+        <v>0.46400000000000002</v>
       </c>
       <c r="K3" s="5">
         <f t="shared" si="2"/>
-        <v>0.41</v>
+        <v>0.47600000000000003</v>
       </c>
       <c r="L3" s="5">
         <f t="shared" si="2"/>
-        <v>0.43</v>
+        <v>0.48800000000000004</v>
       </c>
       <c r="M3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="N3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="O3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="P3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="Q3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="R3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="S3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="T3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="U3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="V3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="W3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="X3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="Y3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="Z3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AA3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AB3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AC3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AD3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AE3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AF3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AG3" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.35">
@@ -15655,131 +15653,131 @@
       </c>
       <c r="B4" s="5">
         <f t="shared" ref="B4:B7" si="3">B3</f>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="C4" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="D4" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="E4" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="G4" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="I4" s="5">
         <f t="shared" si="2"/>
-        <v>0.37</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="J4" s="5">
         <f t="shared" si="2"/>
-        <v>0.39</v>
+        <v>0.46400000000000002</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" si="2"/>
-        <v>0.41</v>
+        <v>0.47600000000000003</v>
       </c>
       <c r="L4" s="5">
         <f t="shared" si="2"/>
-        <v>0.43</v>
+        <v>0.48800000000000004</v>
       </c>
       <c r="M4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="N4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="O4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="P4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="Q4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="R4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="S4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="T4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="U4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="V4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="W4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="X4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="Y4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="Z4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AA4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AB4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AC4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AD4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AE4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AF4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AG4" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.35">
@@ -15788,131 +15786,131 @@
       </c>
       <c r="B5" s="5">
         <f t="shared" si="3"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="C5" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="D5" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="G5" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="H5" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="I5" s="5">
         <f t="shared" si="2"/>
-        <v>0.37</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" si="2"/>
-        <v>0.39</v>
+        <v>0.46400000000000002</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" si="2"/>
-        <v>0.41</v>
+        <v>0.47600000000000003</v>
       </c>
       <c r="L5" s="5">
         <f t="shared" si="2"/>
-        <v>0.43</v>
+        <v>0.48800000000000004</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="N5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="O5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="P5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="Q5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="R5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="S5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="T5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="U5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="V5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="W5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="X5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="Y5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="Z5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AA5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AB5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AC5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AD5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AE5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AF5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AG5" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.35">
@@ -15921,131 +15919,131 @@
       </c>
       <c r="B6" s="5">
         <f t="shared" si="3"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="C6" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="D6" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="I6" s="5">
         <f t="shared" si="2"/>
-        <v>0.37</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="2"/>
-        <v>0.39</v>
+        <v>0.46400000000000002</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="2"/>
-        <v>0.41</v>
+        <v>0.47600000000000003</v>
       </c>
       <c r="L6" s="5">
         <f t="shared" si="2"/>
-        <v>0.43</v>
+        <v>0.48800000000000004</v>
       </c>
       <c r="M6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="N6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="O6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="P6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="Q6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="R6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="S6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="T6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="U6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="V6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="W6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="X6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="Y6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="Z6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AA6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AB6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AC6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AD6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AE6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AF6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AG6" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.35">
@@ -16054,131 +16052,131 @@
       </c>
       <c r="B7" s="5">
         <f t="shared" si="3"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="C7" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="D7" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="2"/>
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
       <c r="I7" s="5">
         <f t="shared" si="2"/>
-        <v>0.37</v>
+        <v>0.45200000000000001</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="2"/>
-        <v>0.39</v>
+        <v>0.46400000000000002</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="2"/>
-        <v>0.41</v>
+        <v>0.47600000000000003</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" si="2"/>
-        <v>0.43</v>
+        <v>0.48800000000000004</v>
       </c>
       <c r="M7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="N7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="O7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="P7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="Q7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="R7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="S7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="T7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="U7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="V7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="W7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="X7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="Y7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="Z7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AA7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AB7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AC7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AD7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AE7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AF7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="AG7" s="5">
         <f t="shared" si="2"/>
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>